<commit_message>
removed now empty 3rd LOINC column that previously held incorrect hemoglobin mappings
</commit_message>
<xml_diff>
--- a/HCV Target Data Dictionary.xlsx
+++ b/HCV Target Data Dictionary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3860" uniqueCount="1302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3737" uniqueCount="1302">
   <si>
     <t>redcap_field_name</t>
   </si>
@@ -4010,8 +4010,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4037,11 +4041,15 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4371,10 +4379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4386,12 +4394,10 @@
     <col min="9" max="9" width="41.6640625" customWidth="1"/>
     <col min="11" max="11" width="29.83203125" customWidth="1"/>
     <col min="12" max="12" width="52.6640625" customWidth="1"/>
-    <col min="14" max="14" width="21.5" customWidth="1"/>
-    <col min="15" max="15" width="27" customWidth="1"/>
-    <col min="16" max="16" width="20.1640625" customWidth="1"/>
+    <col min="13" max="13" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="12.75" customHeight="1">
+    <row r="1" spans="1:14" ht="12.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>1294</v>
       </c>
@@ -4429,22 +4435,13 @@
         <v>23</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>24</v>
+        <v>1299</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>1299</v>
-      </c>
-      <c r="Q1" s="5" t="s">
         <v>1300</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="12.75" customHeight="1">
+    <row r="2" spans="1:14" ht="12.75" customHeight="1">
       <c r="A2" t="s">
         <v>445</v>
       </c>
@@ -4487,17 +4484,8 @@
       <c r="N2" t="s">
         <v>1301</v>
       </c>
-      <c r="O2" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P2" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="3" spans="1:14" ht="12.75" customHeight="1">
       <c r="A3" t="s">
         <v>451</v>
       </c>
@@ -4540,17 +4528,8 @@
       <c r="N3" t="s">
         <v>1301</v>
       </c>
-      <c r="O3" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P3" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="4" spans="1:14" ht="12.75" customHeight="1">
       <c r="A4" t="s">
         <v>457</v>
       </c>
@@ -4593,17 +4572,8 @@
       <c r="N4" t="s">
         <v>1301</v>
       </c>
-      <c r="O4" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="5" spans="1:14" ht="12.75" customHeight="1">
       <c r="A5" t="s">
         <v>467</v>
       </c>
@@ -4646,17 +4616,8 @@
       <c r="N5" t="s">
         <v>1301</v>
       </c>
-      <c r="O5" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P5" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="6" spans="1:14" ht="12.75" customHeight="1">
       <c r="A6" t="s">
         <v>475</v>
       </c>
@@ -4699,17 +4660,8 @@
       <c r="N6" t="s">
         <v>1301</v>
       </c>
-      <c r="O6" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P6" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="7" spans="1:14" ht="12.75" customHeight="1">
       <c r="A7" t="s">
         <v>484</v>
       </c>
@@ -4752,17 +4704,8 @@
       <c r="N7" t="s">
         <v>1301</v>
       </c>
-      <c r="O7" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P7" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="8" spans="1:14" ht="12.75" customHeight="1">
       <c r="A8" t="s">
         <v>492</v>
       </c>
@@ -4805,17 +4748,8 @@
       <c r="N8" t="s">
         <v>1301</v>
       </c>
-      <c r="O8" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P8" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="9" spans="1:14" ht="12.75" customHeight="1">
       <c r="A9" t="s">
         <v>501</v>
       </c>
@@ -4858,17 +4792,8 @@
       <c r="N9" t="s">
         <v>1301</v>
       </c>
-      <c r="O9" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P9" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="10" spans="1:14" ht="12.75" customHeight="1">
       <c r="A10" t="s">
         <v>509</v>
       </c>
@@ -4911,17 +4836,8 @@
       <c r="N10" t="s">
         <v>1301</v>
       </c>
-      <c r="O10" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P10" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="11" spans="1:14" ht="12.75" customHeight="1">
       <c r="A11" t="s">
         <v>518</v>
       </c>
@@ -4964,17 +4880,8 @@
       <c r="N11" t="s">
         <v>1301</v>
       </c>
-      <c r="O11" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P11" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="12" spans="1:14" ht="12.75" customHeight="1">
       <c r="A12" t="s">
         <v>525</v>
       </c>
@@ -5017,17 +4924,8 @@
       <c r="N12" t="s">
         <v>1301</v>
       </c>
-      <c r="O12" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P12" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="13" spans="1:14" ht="12.75" customHeight="1">
       <c r="A13" t="s">
         <v>534</v>
       </c>
@@ -5070,17 +4968,8 @@
       <c r="N13" t="s">
         <v>1301</v>
       </c>
-      <c r="O13" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P13" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="14" spans="1:14" ht="12.75" customHeight="1">
       <c r="A14" t="s">
         <v>541</v>
       </c>
@@ -5123,17 +5012,8 @@
       <c r="N14" t="s">
         <v>1301</v>
       </c>
-      <c r="O14" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P14" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="15" spans="1:14" ht="12.75" customHeight="1">
       <c r="A15" t="s">
         <v>550</v>
       </c>
@@ -5161,14 +5041,14 @@
       <c r="I15" t="s">
         <v>560</v>
       </c>
-      <c r="P15" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="12.75" customHeight="1">
+      <c r="M15" t="s">
+        <v>1301</v>
+      </c>
+      <c r="N15" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="12.75" customHeight="1">
       <c r="A16" t="s">
         <v>561</v>
       </c>
@@ -5211,17 +5091,8 @@
       <c r="N16" t="s">
         <v>1301</v>
       </c>
-      <c r="O16" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P16" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="17" spans="1:14" ht="12.75" customHeight="1">
       <c r="A17" t="s">
         <v>568</v>
       </c>
@@ -5264,17 +5135,8 @@
       <c r="N17" t="s">
         <v>1301</v>
       </c>
-      <c r="O17" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P17" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="18" spans="1:14" ht="12.75" customHeight="1">
       <c r="A18" t="s">
         <v>573</v>
       </c>
@@ -5317,17 +5179,8 @@
       <c r="N18" t="s">
         <v>1301</v>
       </c>
-      <c r="O18" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P18" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="19" spans="1:14" ht="12.75" customHeight="1">
       <c r="A19" t="s">
         <v>579</v>
       </c>
@@ -5370,17 +5223,8 @@
       <c r="N19" t="s">
         <v>1301</v>
       </c>
-      <c r="O19" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P19" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="20" spans="1:14" ht="12.75" customHeight="1">
       <c r="A20" t="s">
         <v>588</v>
       </c>
@@ -5423,17 +5267,8 @@
       <c r="N20" t="s">
         <v>1301</v>
       </c>
-      <c r="O20" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P20" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="21" spans="1:14" ht="12.75" customHeight="1">
       <c r="A21" t="s">
         <v>594</v>
       </c>
@@ -5476,17 +5311,8 @@
       <c r="N21" t="s">
         <v>1301</v>
       </c>
-      <c r="O21" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P21" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="22" spans="1:14" ht="12.75" customHeight="1">
       <c r="A22" t="s">
         <v>603</v>
       </c>
@@ -5529,17 +5355,8 @@
       <c r="N22" t="s">
         <v>1301</v>
       </c>
-      <c r="O22" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P22" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="23" spans="1:14" ht="12.75" customHeight="1">
       <c r="A23" t="s">
         <v>608</v>
       </c>
@@ -5582,17 +5399,8 @@
       <c r="N23" t="s">
         <v>1301</v>
       </c>
-      <c r="O23" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P23" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="24" spans="1:14" ht="12.75" customHeight="1">
       <c r="A24" t="s">
         <v>617</v>
       </c>
@@ -5635,17 +5443,8 @@
       <c r="N24" t="s">
         <v>1301</v>
       </c>
-      <c r="O24" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P24" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="25" spans="1:14" ht="12.75" customHeight="1">
       <c r="A25" t="s">
         <v>622</v>
       </c>
@@ -5688,17 +5487,8 @@
       <c r="N25" t="s">
         <v>1301</v>
       </c>
-      <c r="O25" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P25" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="26" spans="1:14" ht="12.75" customHeight="1">
       <c r="A26" t="s">
         <v>631</v>
       </c>
@@ -5741,17 +5531,8 @@
       <c r="N26" t="s">
         <v>1301</v>
       </c>
-      <c r="O26" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P26" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="27" spans="1:14" ht="12.75" customHeight="1">
       <c r="A27" t="s">
         <v>635</v>
       </c>
@@ -5794,17 +5575,8 @@
       <c r="N27" t="s">
         <v>1301</v>
       </c>
-      <c r="O27" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P27" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="28" spans="1:14" ht="12.75" customHeight="1">
       <c r="A28" t="s">
         <v>644</v>
       </c>
@@ -5847,17 +5619,8 @@
       <c r="N28" t="s">
         <v>1301</v>
       </c>
-      <c r="O28" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P28" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="29" spans="1:14" ht="12.75" customHeight="1">
       <c r="A29" t="s">
         <v>648</v>
       </c>
@@ -5900,17 +5663,8 @@
       <c r="N29" t="s">
         <v>1301</v>
       </c>
-      <c r="O29" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P29" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="30" spans="1:14" ht="12.75" customHeight="1">
       <c r="A30" t="s">
         <v>657</v>
       </c>
@@ -5953,17 +5707,8 @@
       <c r="N30" t="s">
         <v>1301</v>
       </c>
-      <c r="O30" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P30" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="31" spans="1:14" ht="12.75" customHeight="1">
       <c r="A31" t="s">
         <v>663</v>
       </c>
@@ -6006,17 +5751,8 @@
       <c r="N31" t="s">
         <v>1301</v>
       </c>
-      <c r="O31" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P31" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="32" spans="1:14" ht="12.75" customHeight="1">
       <c r="A32" t="s">
         <v>672</v>
       </c>
@@ -6059,17 +5795,8 @@
       <c r="N32" t="s">
         <v>1301</v>
       </c>
-      <c r="O32" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P32" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="33" spans="1:14" ht="12.75" customHeight="1">
       <c r="A33" t="s">
         <v>678</v>
       </c>
@@ -6112,17 +5839,8 @@
       <c r="N33" t="s">
         <v>1301</v>
       </c>
-      <c r="O33" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P33" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="34" spans="1:14" ht="12.75" customHeight="1">
       <c r="A34" t="s">
         <v>687</v>
       </c>
@@ -6165,17 +5883,8 @@
       <c r="N34" t="s">
         <v>1301</v>
       </c>
-      <c r="O34" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P34" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="35" spans="1:14" ht="12.75" customHeight="1">
       <c r="A35" t="s">
         <v>693</v>
       </c>
@@ -6218,17 +5927,8 @@
       <c r="N35" t="s">
         <v>1301</v>
       </c>
-      <c r="O35" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P35" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="36" spans="1:14" ht="12.75" customHeight="1">
       <c r="A36" t="s">
         <v>700</v>
       </c>
@@ -6271,17 +5971,8 @@
       <c r="N36" t="s">
         <v>1301</v>
       </c>
-      <c r="O36" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P36" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="37" spans="1:14" ht="12.75" customHeight="1">
       <c r="A37" t="s">
         <v>705</v>
       </c>
@@ -6324,17 +6015,8 @@
       <c r="N37" t="s">
         <v>1301</v>
       </c>
-      <c r="O37" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P37" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="38" spans="1:14" ht="12.75" customHeight="1">
       <c r="A38" t="s">
         <v>721</v>
       </c>
@@ -6377,17 +6059,8 @@
       <c r="N38" t="s">
         <v>1301</v>
       </c>
-      <c r="O38" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P38" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="39" spans="1:14" ht="12.75" customHeight="1">
       <c r="A39" t="s">
         <v>723</v>
       </c>
@@ -6430,17 +6103,8 @@
       <c r="N39" t="s">
         <v>1301</v>
       </c>
-      <c r="O39" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P39" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="40" spans="1:14" ht="12.75" customHeight="1">
       <c r="A40" t="s">
         <v>728</v>
       </c>
@@ -6483,17 +6147,8 @@
       <c r="N40" t="s">
         <v>1301</v>
       </c>
-      <c r="O40" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P40" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="41" spans="1:14" ht="12.75" customHeight="1">
       <c r="A41" t="s">
         <v>733</v>
       </c>
@@ -6536,17 +6191,8 @@
       <c r="N41" t="s">
         <v>1301</v>
       </c>
-      <c r="O41" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P41" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" ht="12.75" customHeight="1">
+    </row>
+    <row r="42" spans="1:14" ht="12.75" customHeight="1">
       <c r="A42" t="s">
         <v>735</v>
       </c>
@@ -6587,15 +6233,6 @@
         <v>1301</v>
       </c>
       <c r="N42" t="s">
-        <v>1301</v>
-      </c>
-      <c r="O42" t="s">
-        <v>1301</v>
-      </c>
-      <c r="P42" t="s">
-        <v>1301</v>
-      </c>
-      <c r="Q42" t="s">
         <v>1301</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new, alternate LOINC value for ALT
</commit_message>
<xml_diff>
--- a/HCV Target Data Dictionary.xlsx
+++ b/HCV Target Data Dictionary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3737" uniqueCount="1302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3737" uniqueCount="1304">
   <si>
     <t>redcap_field_name</t>
   </si>
@@ -3926,6 +3926,12 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>1744-2</t>
+  </si>
+  <si>
+    <t>Alanine aminotransferase [Enzymatic activity/​volume] in Serum or Plasma by Without P-5'-P</t>
   </si>
 </sst>
 </file>
@@ -4021,7 +4027,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4038,6 +4044,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4381,8 +4390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" topLeftCell="H13" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5164,11 +5173,11 @@
       <c r="I18" t="s">
         <v>578</v>
       </c>
-      <c r="J18" t="s">
-        <v>1301</v>
-      </c>
-      <c r="K18" t="s">
-        <v>1301</v>
+      <c r="J18" s="6" t="s">
+        <v>1302</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>1303</v>
       </c>
       <c r="L18" t="s">
         <v>1301</v>

</xml_diff>

<commit_message>
added new LOINC value for Albumin to data dictionary
</commit_message>
<xml_diff>
--- a/HCV Target Data Dictionary.xlsx
+++ b/HCV Target Data Dictionary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3737" uniqueCount="1304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3736" uniqueCount="1306">
   <si>
     <t>redcap_field_name</t>
   </si>
@@ -3932,6 +3932,12 @@
   </si>
   <si>
     <t>Alanine aminotransferase [Enzymatic activity/​volume] in Serum or Plasma by Without P-5'-P</t>
+  </si>
+  <si>
+    <t>61151-7</t>
+  </si>
+  <si>
+    <t>Albumin [Mass/​volume] in Serum or Plasma by Bromocresol green (BCG) dye binding method</t>
   </si>
 </sst>
 </file>
@@ -4390,8 +4396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H13" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4401,7 +4407,7 @@
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
     <col min="8" max="8" width="23.5" customWidth="1"/>
     <col min="9" max="9" width="41.6640625" customWidth="1"/>
-    <col min="11" max="11" width="29.83203125" customWidth="1"/>
+    <col min="11" max="11" width="71.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="52.6640625" customWidth="1"/>
     <col min="13" max="13" width="20.1640625" customWidth="1"/>
   </cols>
@@ -5220,9 +5226,6 @@
       <c r="J19" t="s">
         <v>1301</v>
       </c>
-      <c r="K19" t="s">
-        <v>1301</v>
-      </c>
       <c r="L19" t="s">
         <v>1301</v>
       </c>
@@ -5526,10 +5529,10 @@
         <v>634</v>
       </c>
       <c r="J26" t="s">
-        <v>1301</v>
-      </c>
-      <c r="K26" t="s">
-        <v>1301</v>
+        <v>1304</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>1305</v>
       </c>
       <c r="L26" t="s">
         <v>1301</v>

</xml_diff>

<commit_message>
added one new LOINC value for HCV RNA
</commit_message>
<xml_diff>
--- a/HCV Target Data Dictionary.xlsx
+++ b/HCV Target Data Dictionary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3736" uniqueCount="1306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3732" uniqueCount="1308">
   <si>
     <t>redcap_field_name</t>
   </si>
@@ -3938,6 +3938,12 @@
   </si>
   <si>
     <t>Albumin [Mass/​volume] in Serum or Plasma by Bromocresol green (BCG) dye binding method</t>
+  </si>
+  <si>
+    <t>49380-9</t>
+  </si>
+  <si>
+    <t>Hepatitis C virus RNA [#/​volume] (viral load) in Unspecified specimen by Probe and target amplification method</t>
   </si>
 </sst>
 </file>
@@ -4022,8 +4028,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4056,15 +4066,19 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4396,8 +4410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="J30" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6100,12 +6114,7 @@
       <c r="I39" t="s">
         <v>727</v>
       </c>
-      <c r="J39" t="s">
-        <v>1301</v>
-      </c>
-      <c r="K39" t="s">
-        <v>1301</v>
-      </c>
+      <c r="K39" s="6"/>
       <c r="L39" t="s">
         <v>1301</v>
       </c>
@@ -6145,10 +6154,10 @@
         <v>732</v>
       </c>
       <c r="J40" t="s">
-        <v>1301</v>
-      </c>
-      <c r="K40" t="s">
-        <v>1301</v>
+        <v>1306</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>1307</v>
       </c>
       <c r="L40" t="s">
         <v>1301</v>
@@ -6231,12 +6240,6 @@
       </c>
       <c r="I42" t="s">
         <v>727</v>
-      </c>
-      <c r="J42" t="s">
-        <v>1301</v>
-      </c>
-      <c r="K42" t="s">
-        <v>1301</v>
       </c>
       <c r="L42" t="s">
         <v>1301</v>

</xml_diff>

<commit_message>
Updating Data Dictionary with new HCV Target REDCap variable names.
</commit_message>
<xml_diff>
--- a/HCV Target Data Dictionary.xlsx
+++ b/HCV Target Data Dictionary.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="dataDictionaryforREDI" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3732" uniqueCount="1308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3732" uniqueCount="1349">
   <si>
     <t>redcap_field_name</t>
   </si>
@@ -3944,6 +3944,129 @@
   </si>
   <si>
     <t>Hepatitis C virus RNA [#/​volume] (viral load) in Unspecified specimen by Probe and target amplification method</t>
+  </si>
+  <si>
+    <t>lym_im_lborres</t>
+  </si>
+  <si>
+    <t>lym_im_lborresu</t>
+  </si>
+  <si>
+    <t>alt_im_lborres</t>
+  </si>
+  <si>
+    <t>alt_im_lborresu</t>
+  </si>
+  <si>
+    <t>alb_im_lborres</t>
+  </si>
+  <si>
+    <t>alb_im_lborresu</t>
+  </si>
+  <si>
+    <t>anc_im_lborres</t>
+  </si>
+  <si>
+    <t>anc_im_lborresu</t>
+  </si>
+  <si>
+    <t>ast_im_lborres</t>
+  </si>
+  <si>
+    <t>ast_im_lborresu</t>
+  </si>
+  <si>
+    <t>dbil_im_lborres</t>
+  </si>
+  <si>
+    <t>dbil_im_lborresu</t>
+  </si>
+  <si>
+    <t>tbil_im_lborres</t>
+  </si>
+  <si>
+    <t>tbil_im_lborresu</t>
+  </si>
+  <si>
+    <t>creat_im_lborres</t>
+  </si>
+  <si>
+    <t>creat_im_lborresu</t>
+  </si>
+  <si>
+    <t>gluc_im_lborres</t>
+  </si>
+  <si>
+    <t>gluc_im_lborresu</t>
+  </si>
+  <si>
+    <t>hcv_im_lborres</t>
+  </si>
+  <si>
+    <t>hcv_im_lborresu</t>
+  </si>
+  <si>
+    <t>hcv_im_supplb_hcvquant</t>
+  </si>
+  <si>
+    <t>hcv_im_lbdtc</t>
+  </si>
+  <si>
+    <t>hcv_im_supplb_hcvdtct</t>
+  </si>
+  <si>
+    <t>hemo_im_lborres</t>
+  </si>
+  <si>
+    <t>hemo_im_lborresu</t>
+  </si>
+  <si>
+    <t>inr_im_lborres</t>
+  </si>
+  <si>
+    <t>inr_im_lbdtc</t>
+  </si>
+  <si>
+    <t>lymce_im_lborres</t>
+  </si>
+  <si>
+    <t>lymce_im_lborresu</t>
+  </si>
+  <si>
+    <t>plat_im_lborres</t>
+  </si>
+  <si>
+    <t>plat_im_lborresu</t>
+  </si>
+  <si>
+    <t>k_im_lborres</t>
+  </si>
+  <si>
+    <t>k_im_lborresu</t>
+  </si>
+  <si>
+    <t>wbc_im_lborres</t>
+  </si>
+  <si>
+    <t>wbc_im_lborresu</t>
+  </si>
+  <si>
+    <t>cbc_im_lbdtc</t>
+  </si>
+  <si>
+    <t>neut_im_lborres</t>
+  </si>
+  <si>
+    <t>neut_im_lborresu</t>
+  </si>
+  <si>
+    <t>chem_im_lbdtc</t>
+  </si>
+  <si>
+    <t>sodium_im_lborres</t>
+  </si>
+  <si>
+    <t>sodium_im_lborresu</t>
   </si>
 </sst>
 </file>
@@ -4410,8 +4533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J30" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4472,7 +4595,7 @@
     </row>
     <row r="2" spans="1:14" ht="12.75" customHeight="1">
       <c r="A2" t="s">
-        <v>445</v>
+        <v>1343</v>
       </c>
       <c r="B2" t="s">
         <v>442</v>
@@ -4516,7 +4639,7 @@
     </row>
     <row r="3" spans="1:14" ht="12.75" customHeight="1">
       <c r="A3" t="s">
-        <v>451</v>
+        <v>1341</v>
       </c>
       <c r="B3" t="s">
         <v>442</v>
@@ -4560,7 +4683,7 @@
     </row>
     <row r="4" spans="1:14" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>457</v>
+        <v>1342</v>
       </c>
       <c r="B4" t="s">
         <v>442</v>
@@ -4604,7 +4727,7 @@
     </row>
     <row r="5" spans="1:14" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>467</v>
+        <v>1344</v>
       </c>
       <c r="B5" t="s">
         <v>442</v>
@@ -4648,7 +4771,7 @@
     </row>
     <row r="6" spans="1:14" ht="12.75" customHeight="1">
       <c r="A6" t="s">
-        <v>475</v>
+        <v>1345</v>
       </c>
       <c r="B6" t="s">
         <v>442</v>
@@ -4692,7 +4815,7 @@
     </row>
     <row r="7" spans="1:14" ht="12.75" customHeight="1">
       <c r="A7" t="s">
-        <v>484</v>
+        <v>1314</v>
       </c>
       <c r="B7" t="s">
         <v>442</v>
@@ -4736,7 +4859,7 @@
     </row>
     <row r="8" spans="1:14" ht="12.75" customHeight="1">
       <c r="A8" t="s">
-        <v>492</v>
+        <v>1315</v>
       </c>
       <c r="B8" t="s">
         <v>442</v>
@@ -4780,7 +4903,7 @@
     </row>
     <row r="9" spans="1:14" ht="12.75" customHeight="1">
       <c r="A9" t="s">
-        <v>501</v>
+        <v>1335</v>
       </c>
       <c r="B9" t="s">
         <v>442</v>
@@ -4824,7 +4947,7 @@
     </row>
     <row r="10" spans="1:14" ht="12.75" customHeight="1">
       <c r="A10" t="s">
-        <v>509</v>
+        <v>1336</v>
       </c>
       <c r="B10" t="s">
         <v>442</v>
@@ -4868,7 +4991,7 @@
     </row>
     <row r="11" spans="1:14" ht="12.75" customHeight="1">
       <c r="A11" t="s">
-        <v>518</v>
+        <v>1308</v>
       </c>
       <c r="B11" t="s">
         <v>442</v>
@@ -4912,7 +5035,7 @@
     </row>
     <row r="12" spans="1:14" ht="12.75" customHeight="1">
       <c r="A12" t="s">
-        <v>525</v>
+        <v>1309</v>
       </c>
       <c r="B12" t="s">
         <v>442</v>
@@ -4956,7 +5079,7 @@
     </row>
     <row r="13" spans="1:14" ht="12.75" customHeight="1">
       <c r="A13" t="s">
-        <v>534</v>
+        <v>1337</v>
       </c>
       <c r="B13" t="s">
         <v>442</v>
@@ -5000,7 +5123,7 @@
     </row>
     <row r="14" spans="1:14" ht="12.75" customHeight="1">
       <c r="A14" t="s">
-        <v>541</v>
+        <v>1338</v>
       </c>
       <c r="B14" t="s">
         <v>442</v>
@@ -5044,7 +5167,7 @@
     </row>
     <row r="15" spans="1:14" ht="12.75" customHeight="1">
       <c r="A15" t="s">
-        <v>550</v>
+        <v>1331</v>
       </c>
       <c r="B15" t="s">
         <v>442</v>
@@ -5079,7 +5202,7 @@
     </row>
     <row r="16" spans="1:14" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>561</v>
+        <v>1332</v>
       </c>
       <c r="B16" t="s">
         <v>442</v>
@@ -5123,7 +5246,7 @@
     </row>
     <row r="17" spans="1:14" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>568</v>
+        <v>1346</v>
       </c>
       <c r="B17" t="s">
         <v>567</v>
@@ -5167,7 +5290,7 @@
     </row>
     <row r="18" spans="1:14" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>573</v>
+        <v>1310</v>
       </c>
       <c r="B18" t="s">
         <v>567</v>
@@ -5211,7 +5334,7 @@
     </row>
     <row r="19" spans="1:14" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>579</v>
+        <v>1311</v>
       </c>
       <c r="B19" t="s">
         <v>567</v>
@@ -5252,7 +5375,7 @@
     </row>
     <row r="20" spans="1:14" ht="12.75" customHeight="1">
       <c r="A20" t="s">
-        <v>588</v>
+        <v>1316</v>
       </c>
       <c r="B20" t="s">
         <v>567</v>
@@ -5296,7 +5419,7 @@
     </row>
     <row r="21" spans="1:14" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>594</v>
+        <v>1317</v>
       </c>
       <c r="B21" t="s">
         <v>567</v>
@@ -5340,7 +5463,7 @@
     </row>
     <row r="22" spans="1:14" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>603</v>
+        <v>1320</v>
       </c>
       <c r="B22" t="s">
         <v>567</v>
@@ -5384,7 +5507,7 @@
     </row>
     <row r="23" spans="1:14" ht="12.75" customHeight="1">
       <c r="A23" t="s">
-        <v>608</v>
+        <v>1321</v>
       </c>
       <c r="B23" t="s">
         <v>567</v>
@@ -5428,7 +5551,7 @@
     </row>
     <row r="24" spans="1:14" ht="12.75" customHeight="1">
       <c r="A24" t="s">
-        <v>617</v>
+        <v>1318</v>
       </c>
       <c r="B24" t="s">
         <v>567</v>
@@ -5472,7 +5595,7 @@
     </row>
     <row r="25" spans="1:14" ht="12.75" customHeight="1">
       <c r="A25" t="s">
-        <v>622</v>
+        <v>1319</v>
       </c>
       <c r="B25" t="s">
         <v>567</v>
@@ -5516,7 +5639,7 @@
     </row>
     <row r="26" spans="1:14" ht="12.75" customHeight="1">
       <c r="A26" t="s">
-        <v>631</v>
+        <v>1312</v>
       </c>
       <c r="B26" t="s">
         <v>567</v>
@@ -5560,7 +5683,7 @@
     </row>
     <row r="27" spans="1:14" ht="12.75" customHeight="1">
       <c r="A27" t="s">
-        <v>635</v>
+        <v>1313</v>
       </c>
       <c r="B27" t="s">
         <v>567</v>
@@ -5604,7 +5727,7 @@
     </row>
     <row r="28" spans="1:14" ht="12.75" customHeight="1">
       <c r="A28" t="s">
-        <v>644</v>
+        <v>1322</v>
       </c>
       <c r="B28" t="s">
         <v>567</v>
@@ -5648,7 +5771,7 @@
     </row>
     <row r="29" spans="1:14" ht="12.75" customHeight="1">
       <c r="A29" t="s">
-        <v>648</v>
+        <v>1323</v>
       </c>
       <c r="B29" t="s">
         <v>567</v>
@@ -5692,7 +5815,7 @@
     </row>
     <row r="30" spans="1:14" ht="12.75" customHeight="1">
       <c r="A30" t="s">
-        <v>657</v>
+        <v>1324</v>
       </c>
       <c r="B30" t="s">
         <v>567</v>
@@ -5736,7 +5859,7 @@
     </row>
     <row r="31" spans="1:14" ht="12.75" customHeight="1">
       <c r="A31" t="s">
-        <v>663</v>
+        <v>1325</v>
       </c>
       <c r="B31" t="s">
         <v>567</v>
@@ -5780,7 +5903,7 @@
     </row>
     <row r="32" spans="1:14" ht="12.75" customHeight="1">
       <c r="A32" t="s">
-        <v>672</v>
+        <v>1339</v>
       </c>
       <c r="B32" t="s">
         <v>567</v>
@@ -5824,7 +5947,7 @@
     </row>
     <row r="33" spans="1:14" ht="12.75" customHeight="1">
       <c r="A33" t="s">
-        <v>678</v>
+        <v>1340</v>
       </c>
       <c r="B33" t="s">
         <v>567</v>
@@ -5868,7 +5991,7 @@
     </row>
     <row r="34" spans="1:14" ht="12.75" customHeight="1">
       <c r="A34" t="s">
-        <v>687</v>
+        <v>1347</v>
       </c>
       <c r="B34" t="s">
         <v>567</v>
@@ -5912,7 +6035,7 @@
     </row>
     <row r="35" spans="1:14" ht="12.75" customHeight="1">
       <c r="A35" t="s">
-        <v>693</v>
+        <v>1348</v>
       </c>
       <c r="B35" t="s">
         <v>567</v>
@@ -5956,7 +6079,7 @@
     </row>
     <row r="36" spans="1:14" ht="12.75" customHeight="1">
       <c r="A36" t="s">
-        <v>700</v>
+        <v>1334</v>
       </c>
       <c r="B36" t="s">
         <v>699</v>
@@ -6000,7 +6123,7 @@
     </row>
     <row r="37" spans="1:14" ht="12.75" customHeight="1">
       <c r="A37" t="s">
-        <v>705</v>
+        <v>1333</v>
       </c>
       <c r="B37" t="s">
         <v>699</v>
@@ -6044,7 +6167,7 @@
     </row>
     <row r="38" spans="1:14" ht="12.75" customHeight="1">
       <c r="A38" t="s">
-        <v>721</v>
+        <v>1329</v>
       </c>
       <c r="B38" t="s">
         <v>717</v>
@@ -6088,7 +6211,7 @@
     </row>
     <row r="39" spans="1:14" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>723</v>
+        <v>1328</v>
       </c>
       <c r="B39" t="s">
         <v>717</v>
@@ -6127,7 +6250,7 @@
     </row>
     <row r="40" spans="1:14" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>728</v>
+        <v>1326</v>
       </c>
       <c r="B40" t="s">
         <v>717</v>
@@ -6171,7 +6294,7 @@
     </row>
     <row r="41" spans="1:14" ht="12.75" customHeight="1">
       <c r="A41" t="s">
-        <v>733</v>
+        <v>1327</v>
       </c>
       <c r="B41" t="s">
         <v>717</v>
@@ -6215,7 +6338,7 @@
     </row>
     <row r="42" spans="1:14" ht="12.75" customHeight="1">
       <c r="A42" t="s">
-        <v>735</v>
+        <v>1330</v>
       </c>
       <c r="B42" t="s">
         <v>717</v>

</xml_diff>